<commit_message>
menuing, sound, and controls working
</commit_message>
<xml_diff>
--- a/scoringCriteria.xlsx
+++ b/scoringCriteria.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="35">
   <si>
     <t>Criteria</t>
   </si>
@@ -114,6 +114,24 @@
   </si>
   <si>
     <t>Possible</t>
+  </si>
+  <si>
+    <t>DONE</t>
+  </si>
+  <si>
+    <t>?</t>
+  </si>
+  <si>
+    <t>First Milestone</t>
+  </si>
+  <si>
+    <t>player controls</t>
+  </si>
+  <si>
+    <t>obstacles generating</t>
+  </si>
+  <si>
+    <t>60 Points Scaled</t>
   </si>
 </sst>
 </file>
@@ -496,7 +514,7 @@
   <dimension ref="A1:AE28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -504,7 +522,9 @@
     <col min="1" max="1" width="24.6640625" customWidth="1"/>
     <col min="2" max="3" width="10.6640625" customWidth="1"/>
     <col min="4" max="4" width="11.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="16" width="10.6640625" customWidth="1"/>
+    <col min="5" max="5" width="10.6640625" customWidth="1"/>
+    <col min="6" max="6" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="16" width="10.6640625" customWidth="1"/>
     <col min="17" max="17" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="18" max="29" width="10.6640625" customWidth="1"/>
     <col min="30" max="31" width="24.6640625" customWidth="1"/>
@@ -520,6 +540,9 @@
       <c r="D1" t="s">
         <v>2</v>
       </c>
+      <c r="F1" t="s">
+        <v>31</v>
+      </c>
       <c r="AD1" t="s">
         <v>3</v>
       </c>
@@ -537,6 +560,9 @@
       <c r="D2" t="s">
         <v>6</v>
       </c>
+      <c r="F2" t="s">
+        <v>34</v>
+      </c>
       <c r="AD2">
         <v>1</v>
       </c>
@@ -554,6 +580,12 @@
       <c r="D3" t="s">
         <v>6</v>
       </c>
+      <c r="E3" t="s">
+        <v>29</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
       <c r="AD3">
         <v>2</v>
       </c>
@@ -571,6 +603,9 @@
       <c r="D4" t="s">
         <v>6</v>
       </c>
+      <c r="F4" t="s">
+        <v>6</v>
+      </c>
       <c r="AD4">
         <v>3</v>
       </c>
@@ -588,6 +623,12 @@
       <c r="D5" t="s">
         <v>6</v>
       </c>
+      <c r="E5" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" t="s">
+        <v>32</v>
+      </c>
     </row>
     <row r="6" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
@@ -599,6 +640,9 @@
       <c r="D6" t="s">
         <v>6</v>
       </c>
+      <c r="F6" t="s">
+        <v>33</v>
+      </c>
     </row>
     <row r="7" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
@@ -607,6 +651,9 @@
       <c r="B7">
         <v>10</v>
       </c>
+      <c r="E7" t="s">
+        <v>6</v>
+      </c>
     </row>
     <row r="8" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
@@ -618,6 +665,9 @@
       <c r="D8" t="s">
         <v>6</v>
       </c>
+      <c r="E8" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="9" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
@@ -629,6 +679,9 @@
       <c r="D9" t="s">
         <v>6</v>
       </c>
+      <c r="E9" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="10" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
@@ -648,6 +701,9 @@
       <c r="D11" t="s">
         <v>6</v>
       </c>
+      <c r="E11" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="12" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
@@ -659,6 +715,9 @@
       <c r="D12" t="s">
         <v>6</v>
       </c>
+      <c r="E12" t="s">
+        <v>29</v>
+      </c>
     </row>
     <row r="13" spans="1:31" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
@@ -674,6 +733,9 @@
       </c>
       <c r="B14">
         <v>10</v>
+      </c>
+      <c r="E14" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="15" spans="1:31" x14ac:dyDescent="0.15">

</xml_diff>